<commit_message>
Updated input spreadsheet, added reactor.yaml
</commit_message>
<xml_diff>
--- a/pmutt_to_omkm/inputs/NH3_Input_Data.xlsx
+++ b/pmutt_to_omkm/inputs/NH3_Input_Data.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerhard\Dropbox\Milan 2020 MultiscaleModelingWorkshop (1)\WorkshopJupyterNotebooks\pmutt_to_omkm\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerhard\Documents\GitHub\ACS_Workshop_Aug_2023\pmutt_to_omkm\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799FAAA1-2C6D-4620-99E8-2466C569213B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CD33E4-F7B9-4699-AD4F-171D581E25F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="0" windowWidth="28710" windowHeight="15480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="90" yWindow="0" windowWidth="28710" windowHeight="15480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="refs" sheetId="2" r:id="rId1"/>
     <sheet name="species" sheetId="1" r:id="rId2"/>
-    <sheet name="beps" sheetId="7" r:id="rId3"/>
-    <sheet name="phases" sheetId="5" r:id="rId4"/>
-    <sheet name="reactions" sheetId="3" r:id="rId5"/>
-    <sheet name="lateral_interactions" sheetId="6" r:id="rId6"/>
+    <sheet name="reactor" sheetId="8" r:id="rId3"/>
+    <sheet name="beps" sheetId="7" r:id="rId4"/>
+    <sheet name="phases" sheetId="5" r:id="rId5"/>
+    <sheet name="reactions" sheetId="3" r:id="rId6"/>
+    <sheet name="lateral_interactions" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="156">
   <si>
     <t>name</t>
   </si>
@@ -409,6 +410,102 @@
   </si>
   <si>
     <t>Ru(0001) with atoms deleted</t>
+  </si>
+  <si>
+    <t>reactor_type</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>cat_abyv</t>
+  </si>
+  <si>
+    <t>end_time</t>
+  </si>
+  <si>
+    <t>flow_rate</t>
+  </si>
+  <si>
+    <t>transient</t>
+  </si>
+  <si>
+    <t>stepping</t>
+  </si>
+  <si>
+    <t>init_step</t>
+  </si>
+  <si>
+    <t>atol</t>
+  </si>
+  <si>
+    <t>rtol</t>
+  </si>
+  <si>
+    <t>output_format</t>
+  </si>
+  <si>
+    <t>Type of reactor. Accepted options include 'pfr', 'cstr', 'pfr_0d', 'batch'</t>
+  </si>
+  <si>
+    <t>Mode of operation.</t>
+  </si>
+  <si>
+    <t>Volume of reactor (units correspond to length^3 in units sheet)</t>
+  </si>
+  <si>
+    <t>Temperature of reactor in K</t>
+  </si>
+  <si>
+    <t>Pressure of reactor (units correspond to pressure in units sheet)</t>
+  </si>
+  <si>
+    <t>Catalyst surface area to reactor volume ratio (units correspond to 1/length in units sheet)</t>
+  </si>
+  <si>
+    <t>Time taken to converge (units correspond to time in unit sheet)</t>
+  </si>
+  <si>
+    <t>Flow rate (units correspond to length^3/time in units sheet)</t>
+  </si>
+  <si>
+    <t>If True, transient run data will be saved.</t>
+  </si>
+  <si>
+    <t>Type of time stepping to perform during transient runs.</t>
+  </si>
+  <si>
+    <t>Solver option for initial time step taken. Corresponds to time in units sheet.</t>
+  </si>
+  <si>
+    <t>Solver option for absolute tolerance.</t>
+  </si>
+  <si>
+    <t>Solver option for relative tolerance</t>
+  </si>
+  <si>
+    <t>Format to write output formats. Accepted options are 'dat' and 'csv'.</t>
+  </si>
+  <si>
+    <t>cstr</t>
+  </si>
+  <si>
+    <t>isothermal</t>
+  </si>
+  <si>
+    <t>logarithmic</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>temperature_mode</t>
   </si>
 </sst>
 </file>
@@ -911,7 +1008,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -926,7 +1023,6 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1792,7 +1888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BS63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3223,7 +3319,7 @@
       <c r="B17">
         <v>2</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" t="s">
         <v>111</v>
       </c>
       <c r="F17">
@@ -3302,7 +3398,7 @@
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" t="s">
         <v>111</v>
       </c>
       <c r="F18">
@@ -3375,7 +3471,7 @@
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" t="s">
         <v>111</v>
       </c>
       <c r="F19">
@@ -3451,7 +3547,7 @@
       <c r="C20">
         <v>3</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" t="s">
         <v>111</v>
       </c>
       <c r="F20">
@@ -3545,7 +3641,7 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" t="s">
         <v>111</v>
       </c>
       <c r="F21">
@@ -3633,7 +3729,7 @@
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" t="s">
         <v>111</v>
       </c>
       <c r="F22">
@@ -3715,7 +3811,6 @@
       <c r="C23">
         <v>3</v>
       </c>
-      <c r="E23" s="10"/>
       <c r="F23">
         <v>1</v>
       </c>
@@ -3805,7 +3900,6 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="E24" s="10"/>
       <c r="F24">
         <v>1</v>
       </c>
@@ -3889,7 +3983,6 @@
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="E25" s="10"/>
       <c r="F25">
         <v>1</v>
       </c>
@@ -3964,7 +4057,6 @@
       <c r="B26">
         <v>2</v>
       </c>
-      <c r="E26" s="10"/>
       <c r="F26">
         <v>1</v>
       </c>
@@ -5499,6 +5591,153 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76058666-6699-4726-8164-67E37D315FC2}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>900</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1500</v>
+      </c>
+      <c r="G3">
+        <v>50</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>153</v>
+      </c>
+      <c r="K3" s="8">
+        <v>1E-10</v>
+      </c>
+      <c r="L3" s="8">
+        <v>1E-10</v>
+      </c>
+      <c r="M3" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="N3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA3BA1A-334E-44D2-96CB-219546C8DBF5}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -5596,7 +5835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DF76BA-4A75-44F6-9B27-46A6358EAEB9}">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -5726,7 +5965,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB50E3A2-FDBB-4648-8333-2A8A81886E9C}">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -5921,7 +6160,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19551FD-AEAC-4B83-AFF0-1C4D43FB7482}">
   <dimension ref="A1:D12"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated lateral interaction in spreadsheet
</commit_message>
<xml_diff>
--- a/pmutt_to_omkm/inputs/NH3_Input_Data.xlsx
+++ b/pmutt_to_omkm/inputs/NH3_Input_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gerhard\Documents\GitHub\ACS_Workshop_Aug_2023\pmutt_to_omkm\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06A239D-FD81-4513-9897-0EE77C7A4066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D00B090-0BE3-4E87-AA1F-423BDAB1E601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="0" windowWidth="28710" windowHeight="15480" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="315" windowWidth="28710" windowHeight="15480" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="refs" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="162">
   <si>
     <t>name</t>
   </si>
@@ -5857,7 +5857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DF76BA-4A75-44F6-9B27-46A6358EAEB9}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -6209,10 +6209,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B19551FD-AEAC-4B83-AFF0-1C4D43FB7482}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6220,7 +6220,7 @@
     <col min="3" max="3" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
@@ -6233,8 +6233,11 @@
       <c r="D1" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>77</v>
       </c>
@@ -6247,8 +6250,11 @@
       <c r="D2" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>101</v>
       </c>
@@ -6261,8 +6267,11 @@
       <c r="D3">
         <v>-52.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -6275,8 +6284,11 @@
       <c r="D4">
         <v>-17.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -6289,8 +6301,11 @@
       <c r="D5">
         <v>-17.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -6303,8 +6318,11 @@
       <c r="D6">
         <v>-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -6317,8 +6335,11 @@
       <c r="D7">
         <v>-20.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -6331,8 +6352,11 @@
       <c r="D8">
         <v>-52.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -6345,8 +6369,11 @@
       <c r="D9">
         <v>-17.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -6359,8 +6386,11 @@
       <c r="D10">
         <v>-17.7</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -6373,8 +6403,11 @@
       <c r="D11">
         <v>-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -6386,6 +6419,9 @@
       </c>
       <c r="D12">
         <v>-20.7</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>